<commit_message>
docs: Modelo de diseño actualizado y prototipo
</commit_message>
<xml_diff>
--- a/Commmits.xlsx
+++ b/Commmits.xlsx
@@ -176,11 +176,11 @@
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:axId val="445843056"/>
-        <c:axId val="1482703293"/>
+        <c:axId val="1577687518"/>
+        <c:axId val="393821979"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="445843056"/>
+        <c:axId val="1577687518"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -232,10 +232,10 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1482703293"/>
+        <c:crossAx val="393821979"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="1482703293"/>
+        <c:axId val="393821979"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -310,7 +310,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="445843056"/>
+        <c:crossAx val="1577687518"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
@@ -341,7 +341,7 @@
   <xdr:oneCellAnchor>
     <xdr:from>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>561975</xdr:colOff>
+      <xdr:colOff>609600</xdr:colOff>
       <xdr:row>5</xdr:row>
       <xdr:rowOff>95250</xdr:rowOff>
     </xdr:from>
@@ -618,7 +618,7 @@
       </c>
       <c r="C4" s="6">
         <f>SUM(A3:A32)</f>
-        <v>61</v>
+        <v>66</v>
       </c>
     </row>
     <row r="5" ht="15.75" customHeight="1">
@@ -791,10 +791,20 @@
       <c r="G25" s="9"/>
     </row>
     <row r="26" ht="15.75" customHeight="1">
-      <c r="A26" s="6"/>
+      <c r="A26" s="7">
+        <v>1.0</v>
+      </c>
+      <c r="B26" s="8">
+        <v>45946.0</v>
+      </c>
     </row>
     <row r="27" ht="15.75" customHeight="1">
-      <c r="A27" s="6"/>
+      <c r="A27" s="7">
+        <v>4.0</v>
+      </c>
+      <c r="B27" s="8">
+        <v>45947.0</v>
+      </c>
     </row>
     <row r="28" ht="15.75" customHeight="1">
       <c r="A28" s="6"/>

</xml_diff>